<commit_message>
Fixed some incorrect files
</commit_message>
<xml_diff>
--- a/CAD/Parts List.xlsx
+++ b/CAD/Parts List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mryor\Google Drive\Projects\MyRobot\3D models\#MOVEO ENHANCED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mryor\Google Drive\Projects\MyRobot\V0\CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{38F261E2-BAAC-4A6A-97FF-BD71DDE1B32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{1E4ED226-2DD2-4203-886A-8971DF99834A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16905" yWindow="2535" windowWidth="21600" windowHeight="11400" xr2:uid="{B1DC88AF-044A-48C4-9875-12BB1562E420}"/>
+    <workbookView xWindow="-12435" yWindow="6675" windowWidth="21600" windowHeight="11400" xr2:uid="{B1DC88AF-044A-48C4-9875-12BB1562E420}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -930,21 +930,12 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B2607FD9-C706-499C-9FC9-CFC958478A05}" diskRevisions="1" version="2">
-  <header guid="{386D682E-B040-48F9-B313-4989A3B12E7C}" dateTime="2021-06-14T22:20:46" maxSheetId="2" userName="Jack York" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
   <header guid="{B2607FD9-C706-499C-9FC9-CFC958478A05}" dateTime="2021-06-14T22:45:14" maxSheetId="2" userName="Jack York" r:id="rId2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -975,7 +966,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -1278,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEB41AE-D615-4E81-A3CF-5528226F900A}">
   <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1307,718 +1298,832 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D4" s="1">
-        <v>4</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D6" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>225</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>198</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="D7" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>226</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D9" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>188</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D11" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D12" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>175</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D14" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>178</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D15" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D16" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D18" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>160</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D20" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D23" s="1">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>162</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D24" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>186</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D25" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>181</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D27" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>151</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D29" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D30" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D32" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D34" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D36" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D37" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D38" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D39" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D40" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D41" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D42" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D43" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C44" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D44" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D45" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>45</v>
+        <v>171</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D46" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>48</v>
+        <v>221</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C49" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>49</v>
+        <v>229</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="1"/>
+        <v>205</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D51" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>53</v>
+        <v>192</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C54" s="1"/>
+        <v>245</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D54" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>54</v>
+        <v>197</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D55" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D56" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>56</v>
+        <v>196</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D57" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D58" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1">
@@ -2027,34 +2132,36 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>61</v>
+        <v>177</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D62" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1">
@@ -2063,10 +2170,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1">
@@ -2075,154 +2182,176 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D66" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>66</v>
+        <v>174</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D67" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C68" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D68" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C69" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C70" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D70" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C71" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D71" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C72" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D72" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C73" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D73" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C74" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D74" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C75" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D75" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>75</v>
+        <v>191</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C76" s="1"/>
+        <v>166</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>225</v>
+        <v>41</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1">
@@ -2231,58 +2360,58 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1">
@@ -2291,58 +2420,60 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>226</v>
+        <v>92</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>86</v>
+        <v>218</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C87" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="D87" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1">
@@ -2351,58 +2482,58 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>80</v>
+        <v>221</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1">
@@ -2411,34 +2542,34 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>95</v>
+        <v>211</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>86</v>
+        <v>182</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1">
@@ -2447,34 +2578,34 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>88</v>
+        <v>222</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1">
@@ -2483,70 +2614,70 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>91</v>
+        <v>223</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>228</v>
+        <v>96</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1">
@@ -2555,34 +2686,36 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>106</v>
+        <v>220</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C107" s="1"/>
+        <v>254</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D107" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>97</v>
+        <v>228</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1">
@@ -2591,10 +2724,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1">
@@ -2603,58 +2736,60 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>110</v>
+        <v>223</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C111" s="1"/>
+        <v>255</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="D111" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>113</v>
+        <v>210</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>103</v>
+        <v>248</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1">
@@ -2663,118 +2798,110 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>114</v>
+        <v>199</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C116" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D116" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>106</v>
+        <v>194</v>
       </c>
       <c r="D117" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="C118" s="1"/>
       <c r="D118" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C119" s="1"/>
       <c r="D119" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C120" s="1"/>
       <c r="D120" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C121" s="1"/>
       <c r="D121" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C122" s="1"/>
       <c r="D122" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>112</v>
+        <v>243</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>106</v>
@@ -2785,69 +2912,63 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C124" s="1"/>
       <c r="D124" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>124</v>
+        <v>200</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C125" s="1"/>
       <c r="D125" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>125</v>
+        <v>213</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="C126" s="1"/>
       <c r="D126" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>126</v>
+        <v>227</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="D127" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>117</v>
+        <v>256</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="D128" s="1">
         <v>1</v>
@@ -2855,66 +2976,60 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C129" s="1"/>
       <c r="D129" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C130" s="1"/>
       <c r="D130" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="C131" s="1"/>
       <c r="D131" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>121</v>
+        <v>234</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D132" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>122</v>
+        <v>244</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>106</v>
@@ -2923,12 +3038,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>123</v>
+        <v>236</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>106</v>
@@ -2937,12 +3052,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>124</v>
+        <v>231</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>106</v>
@@ -2951,12 +3066,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>125</v>
+        <v>235</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>106</v>
@@ -2965,40 +3080,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>126</v>
+        <v>242</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D137" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>127</v>
+        <v>233</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D138" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>106</v>
@@ -3009,10 +3124,10 @@
     </row>
     <row r="140" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>106</v>
@@ -3023,433 +3138,383 @@
     </row>
     <row r="141" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
+        <v>158</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D141" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>138</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D142" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>156</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D143" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>157</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D144" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
         <v>140</v>
       </c>
-      <c r="B141" s="3" t="s">
+      <c r="B145" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D141" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
-        <v>141</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D142" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
-        <v>142</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D143" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>143</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D144" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <v>144</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="C145" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D145" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>145</v>
+        <v>10</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C146" s="1"/>
       <c r="D146" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>146</v>
+        <v>22</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C147" s="1"/>
       <c r="D147" s="1">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C148" s="1"/>
       <c r="D148" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C149" s="1"/>
       <c r="D149" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>149</v>
+        <v>70</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C150" s="1"/>
       <c r="D150" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>150</v>
+        <v>52</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C151" s="1"/>
       <c r="D151" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C152" s="1"/>
       <c r="D152" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>152</v>
+        <v>23</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C153" s="1"/>
       <c r="D153" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>36</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>42</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <v>153</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D154" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <v>154</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D155" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C156" s="1"/>
       <c r="D156" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C157" s="1"/>
       <c r="D157" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C158" s="1"/>
       <c r="D158" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C159" s="1"/>
       <c r="D159" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>159</v>
+        <v>12</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C160" s="1"/>
       <c r="D160" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C161" s="1"/>
       <c r="D161" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C162" s="1"/>
       <c r="D162" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C163" s="1"/>
       <c r="D163" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>163</v>
+        <v>6</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C164" s="1"/>
       <c r="D164" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>164</v>
+        <v>58</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C165" s="1"/>
       <c r="D165" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>165</v>
+        <v>8</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C166" s="1"/>
       <c r="D166" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>166</v>
+        <v>2</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C167" s="1"/>
       <c r="D167" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C168" s="1"/>
       <c r="D168" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>168</v>
+        <v>31</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C169" s="1"/>
       <c r="D169" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>169</v>
+        <v>30</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C170" s="1"/>
       <c r="D170" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>170</v>
+        <v>216</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>146</v>
+        <v>253</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>106</v>
+        <v>183</v>
       </c>
       <c r="D171" s="1">
         <v>1</v>
@@ -3457,388 +3522,336 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C172" s="1"/>
       <c r="D172" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C173" s="1"/>
       <c r="D173" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>173</v>
+        <v>235</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C174" s="1"/>
       <c r="D174" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>174</v>
+        <v>50</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C175" s="1"/>
       <c r="D175" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>175</v>
+        <v>63</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C176" s="1"/>
       <c r="D176" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>176</v>
+        <v>46</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C177" s="1"/>
       <c r="D177" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C178" s="1"/>
       <c r="D178" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>178</v>
+        <v>37</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C179" s="1"/>
       <c r="D179" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>88</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
-        <v>179</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D180" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="C181" s="1"/>
       <c r="D181" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="C182" s="1"/>
       <c r="D182" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C183" s="1"/>
       <c r="D183" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>183</v>
+        <v>86</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="C184" s="1"/>
       <c r="D184" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>184</v>
+        <v>234</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="C185" s="1"/>
       <c r="D185" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="C186" s="1"/>
       <c r="D186" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>186</v>
+        <v>110</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C187" s="1"/>
       <c r="D187" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>162</v>
+        <v>246</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D188" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C189" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="C189" s="1"/>
       <c r="D189" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C190" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="C190" s="1"/>
       <c r="D190" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C191" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="C191" s="1"/>
       <c r="D191" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C192" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="C192" s="1"/>
       <c r="D192" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C193" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="C193" s="1"/>
       <c r="D193" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C194" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="C194" s="1"/>
       <c r="D194" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>194</v>
+        <v>73</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C195" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C195" s="1"/>
       <c r="D195" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>195</v>
+        <v>236</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C196" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="C196" s="1"/>
       <c r="D196" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="C197" s="1"/>
       <c r="D197" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="C198" s="1"/>
       <c r="D198" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>198</v>
+        <v>91</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1">
@@ -3847,46 +3860,46 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>172</v>
+        <v>20</v>
       </c>
       <c r="C200" s="1"/>
       <c r="D200" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>200</v>
+        <v>64</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>173</v>
+        <v>61</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>201</v>
+        <v>77</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>174</v>
+        <v>225</v>
       </c>
       <c r="C202" s="1"/>
       <c r="D202" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>202</v>
+        <v>98</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="C203" s="1"/>
       <c r="D203" s="1">
@@ -3895,22 +3908,22 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>203</v>
+        <v>103</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>176</v>
+        <v>93</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C205" s="1"/>
       <c r="D205" s="1">
@@ -3919,10 +3932,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C206" s="1"/>
       <c r="D206" s="1">
@@ -3931,10 +3944,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="C207" s="1"/>
       <c r="D207" s="1">
@@ -3943,22 +3956,22 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>207</v>
+        <v>96</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>180</v>
+        <v>87</v>
       </c>
       <c r="C208" s="1"/>
       <c r="D208" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>208</v>
+        <v>111</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>247</v>
+        <v>101</v>
       </c>
       <c r="C209" s="1"/>
       <c r="D209" s="1">
@@ -3967,34 +3980,34 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>209</v>
+        <v>97</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>181</v>
+        <v>88</v>
       </c>
       <c r="C210" s="1"/>
       <c r="D210" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>210</v>
+        <v>24</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>248</v>
+        <v>26</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>211</v>
+        <v>40</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="1">
@@ -4003,10 +4016,10 @@
     </row>
     <row r="213" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>212</v>
+        <v>18</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="C213" s="1"/>
       <c r="D213" s="1">
@@ -4015,292 +4028,268 @@
     </row>
     <row r="214" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>213</v>
+        <v>48</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="C214" s="1"/>
       <c r="D214" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C215" s="1"/>
+        <v>188</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="D215" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C216" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="D216" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>183</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C217" s="1"/>
       <c r="D217" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>185</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="C218" s="1"/>
       <c r="D218" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>218</v>
+        <v>66</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>187</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C219" s="1"/>
       <c r="D219" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="D220" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>220</v>
+        <v>16</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>190</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C221" s="1"/>
       <c r="D221" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>221</v>
+        <v>9</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>192</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C222" s="1"/>
       <c r="D222" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>222</v>
+        <v>35</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>194</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C223" s="1"/>
       <c r="D223" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>223</v>
+        <v>51</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>195</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C224" s="1"/>
       <c r="D224" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>224</v>
+        <v>21</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>197</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C225" s="1"/>
       <c r="D225" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>199</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C226" s="1"/>
       <c r="D226" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>226</v>
+        <v>54</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>201</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C227" s="1"/>
       <c r="D227" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>227</v>
+        <v>26</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>203</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="C228" s="1"/>
       <c r="D228" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>228</v>
+        <v>43</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>204</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C229" s="1"/>
       <c r="D229" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>229</v>
+        <v>71</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>206</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C230" s="1"/>
       <c r="D230" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>230</v>
+        <v>55</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>208</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C231" s="1"/>
       <c r="D231" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>209</v>
+        <v>249</v>
       </c>
       <c r="C232" s="1"/>
       <c r="D232" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>232</v>
+        <v>99</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>210</v>
+        <v>90</v>
       </c>
       <c r="C233" s="1"/>
       <c r="D233" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>233</v>
+        <v>89</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>257</v>
+        <v>80</v>
       </c>
       <c r="C234" s="1"/>
       <c r="D234" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>234</v>
+        <v>105</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>211</v>
+        <v>95</v>
       </c>
       <c r="C235" s="1"/>
       <c r="D235" s="1">
@@ -4309,70 +4298,72 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C236" s="1"/>
+        <v>196</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="D236" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>213</v>
+        <v>257</v>
       </c>
       <c r="C237" s="1"/>
       <c r="D237" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>237</v>
+        <v>112</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>214</v>
+        <v>102</v>
       </c>
       <c r="C238" s="1"/>
       <c r="D238" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>238</v>
+        <v>79</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>258</v>
+        <v>72</v>
       </c>
       <c r="C239" s="1"/>
       <c r="D239" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>239</v>
+        <v>81</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>259</v>
+        <v>74</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>215</v>
+        <v>81</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1">
@@ -4380,6 +4371,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D241">
+    <sortCondition ref="B2:B241"/>
+  </sortState>
   <customSheetViews>
     <customSheetView guid="{EEBA1989-C29F-418B-81D7-F430F400D75A}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4389,4 +4383,251 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
+  <rowSortMap ref="A2:XFD241" count="240">
+    <row newVal="1" oldVal="183"/>
+    <row newVal="2" oldVal="128"/>
+    <row newVal="3" oldVal="130"/>
+    <row newVal="4" oldVal="131"/>
+    <row newVal="5" oldVal="184"/>
+    <row newVal="6" oldVal="225"/>
+    <row newVal="7" oldVal="226"/>
+    <row newVal="8" oldVal="189"/>
+    <row newVal="9" oldVal="188"/>
+    <row newVal="10" oldVal="165"/>
+    <row newVal="11" oldVal="132"/>
+    <row newVal="12" oldVal="126"/>
+    <row newVal="13" oldVal="175"/>
+    <row newVal="14" oldVal="178"/>
+    <row newVal="15" oldVal="133"/>
+    <row newVal="16" oldVal="182"/>
+    <row newVal="17" oldVal="176"/>
+    <row newVal="18" oldVal="120"/>
+    <row newVal="19" oldVal="185"/>
+    <row newVal="20" oldVal="148"/>
+    <row newVal="21" oldVal="118"/>
+    <row newVal="22" oldVal="190"/>
+    <row newVal="23" oldVal="187"/>
+    <row newVal="24" oldVal="186"/>
+    <row newVal="25" oldVal="181"/>
+    <row newVal="26" oldVal="134"/>
+    <row newVal="27" oldVal="151"/>
+    <row newVal="28" oldVal="136"/>
+    <row newVal="29" oldVal="164"/>
+    <row newVal="30" oldVal="152"/>
+    <row newVal="31" oldVal="137"/>
+    <row newVal="32" oldVal="135"/>
+    <row newVal="33" oldVal="129"/>
+    <row newVal="34" oldVal="163"/>
+    <row newVal="35" oldVal="146"/>
+    <row newVal="36" oldVal="147"/>
+    <row newVal="37" oldVal="166"/>
+    <row newVal="38" oldVal="193"/>
+    <row newVal="39" oldVal="143"/>
+    <row newVal="40" oldVal="121"/>
+    <row newVal="41" oldVal="145"/>
+    <row newVal="42" oldVal="172"/>
+    <row newVal="43" oldVal="144"/>
+    <row newVal="44" oldVal="180"/>
+    <row newVal="45" oldVal="171"/>
+    <row newVal="46" oldVal="162"/>
+    <row newVal="47" oldVal="124"/>
+    <row newVal="48" oldVal="221"/>
+    <row newVal="49" oldVal="229"/>
+    <row newVal="50" oldVal="168"/>
+    <row newVal="51" oldVal="127"/>
+    <row newVal="52" oldVal="116"/>
+    <row newVal="53" oldVal="192"/>
+    <row newVal="54" oldVal="197"/>
+    <row newVal="55" oldVal="195"/>
+    <row newVal="56" oldVal="196"/>
+    <row newVal="57" oldVal="125"/>
+    <row newVal="58" oldVal="27"/>
+    <row newVal="59" oldVal="1"/>
+    <row newVal="60" oldVal="75"/>
+    <row newVal="61" oldVal="177"/>
+    <row newVal="62" oldVal="7"/>
+    <row newVal="63" oldVal="32"/>
+    <row newVal="64" oldVal="33"/>
+    <row newVal="65" oldVal="173"/>
+    <row newVal="66" oldVal="174"/>
+    <row newVal="67" oldVal="169"/>
+    <row newVal="68" oldVal="170"/>
+    <row newVal="69" oldVal="119"/>
+    <row newVal="70" oldVal="142"/>
+    <row newVal="71" oldVal="141"/>
+    <row newVal="72" oldVal="123"/>
+    <row newVal="73" oldVal="122"/>
+    <row newVal="74" oldVal="117"/>
+    <row newVal="75" oldVal="191"/>
+    <row newVal="76" oldVal="34"/>
+    <row newVal="77" oldVal="41"/>
+    <row newVal="78" oldVal="44"/>
+    <row newVal="79" oldVal="45"/>
+    <row newVal="80" oldVal="49"/>
+    <row newVal="81" oldVal="57"/>
+    <row newVal="82" oldVal="60"/>
+    <row newVal="83" oldVal="61"/>
+    <row newVal="84" oldVal="5"/>
+    <row newVal="85" oldVal="102"/>
+    <row newVal="86" oldVal="218"/>
+    <row newVal="87" oldVal="56"/>
+    <row newVal="88" oldVal="72"/>
+    <row newVal="89" oldVal="53"/>
+    <row newVal="90" oldVal="13"/>
+    <row newVal="91" oldVal="3"/>
+    <row newVal="92" oldVal="104"/>
+    <row newVal="93" oldVal="19"/>
+    <row newVal="94" oldVal="20"/>
+    <row newVal="95" oldVal="211"/>
+    <row newVal="96" oldVal="25"/>
+    <row newVal="97" oldVal="67"/>
+    <row newVal="98" oldVal="65"/>
+    <row newVal="99" oldVal="68"/>
+    <row newVal="100" oldVal="69"/>
+    <row newVal="101" oldVal="106"/>
+    <row newVal="102" oldVal="114"/>
+    <row newVal="103" oldVal="94"/>
+    <row newVal="104" oldVal="95"/>
+    <row newVal="105" oldVal="47"/>
+    <row newVal="106" oldVal="220"/>
+    <row newVal="107" oldVal="101"/>
+    <row newVal="108" oldVal="92"/>
+    <row newVal="109" oldVal="100"/>
+    <row newVal="110" oldVal="223"/>
+    <row newVal="111" oldVal="115"/>
+    <row newVal="112" oldVal="87"/>
+    <row newVal="113" oldVal="210"/>
+    <row newVal="114" oldVal="199"/>
+    <row newVal="115" oldVal="161"/>
+    <row newVal="116" oldVal="222"/>
+    <row newVal="117" oldVal="239"/>
+    <row newVal="118" oldVal="113"/>
+    <row newVal="119" oldVal="107"/>
+    <row newVal="120" oldVal="108"/>
+    <row newVal="121" oldVal="109"/>
+    <row newVal="122" oldVal="167"/>
+    <row newVal="123" oldVal="198"/>
+    <row newVal="124" oldVal="200"/>
+    <row newVal="125" oldVal="213"/>
+    <row newVal="126" oldVal="227"/>
+    <row newVal="127" oldVal="228"/>
+    <row newVal="128" oldVal="84"/>
+    <row newVal="129" oldVal="82"/>
+    <row newVal="130" oldVal="85"/>
+    <row newVal="131" oldVal="150"/>
+    <row newVal="132" oldVal="179"/>
+    <row newVal="133" oldVal="154"/>
+    <row newVal="134" oldVal="139"/>
+    <row newVal="135" oldVal="153"/>
+    <row newVal="136" oldVal="160"/>
+    <row newVal="137" oldVal="149"/>
+    <row newVal="138" oldVal="155"/>
+    <row newVal="139" oldVal="159"/>
+    <row newVal="140" oldVal="158"/>
+    <row newVal="141" oldVal="138"/>
+    <row newVal="142" oldVal="156"/>
+    <row newVal="143" oldVal="157"/>
+    <row newVal="144" oldVal="140"/>
+    <row newVal="145" oldVal="10"/>
+    <row newVal="146" oldVal="22"/>
+    <row newVal="147" oldVal="38"/>
+    <row newVal="148" oldVal="59"/>
+    <row newVal="149" oldVal="70"/>
+    <row newVal="150" oldVal="52"/>
+    <row newVal="151" oldVal="62"/>
+    <row newVal="152" oldVal="23"/>
+    <row newVal="153" oldVal="36"/>
+    <row newVal="154" oldVal="42"/>
+    <row newVal="155" oldVal="29"/>
+    <row newVal="156" oldVal="11"/>
+    <row newVal="157" oldVal="15"/>
+    <row newVal="158" oldVal="39"/>
+    <row newVal="159" oldVal="12"/>
+    <row newVal="160" oldVal="14"/>
+    <row newVal="161" oldVal="78"/>
+    <row newVal="162" oldVal="28"/>
+    <row newVal="163" oldVal="6"/>
+    <row newVal="164" oldVal="58"/>
+    <row newVal="165" oldVal="8"/>
+    <row newVal="166" oldVal="2"/>
+    <row newVal="167" oldVal="80"/>
+    <row newVal="168" oldVal="31"/>
+    <row newVal="169" oldVal="30"/>
+    <row newVal="170" oldVal="216"/>
+    <row newVal="171" oldVal="93"/>
+    <row newVal="172" oldVal="83"/>
+    <row newVal="173" oldVal="235"/>
+    <row newVal="174" oldVal="50"/>
+    <row newVal="175" oldVal="63"/>
+    <row newVal="176" oldVal="46"/>
+    <row newVal="177" oldVal="76"/>
+    <row newVal="178" oldVal="37"/>
+    <row newVal="179" oldVal="88"/>
+    <row newVal="180" oldVal="214"/>
+    <row newVal="181" oldVal="215"/>
+    <row newVal="182" oldVal="201"/>
+    <row newVal="183" oldVal="86"/>
+    <row newVal="184" oldVal="234"/>
+    <row newVal="185" oldVal="231"/>
+    <row newVal="186" oldVal="110"/>
+    <row newVal="187" oldVal="194"/>
+    <row newVal="188" oldVal="204"/>
+    <row newVal="189" oldVal="209"/>
+    <row newVal="190" oldVal="205"/>
+    <row newVal="191" oldVal="206"/>
+    <row newVal="192" oldVal="207"/>
+    <row newVal="193" oldVal="208"/>
+    <row newVal="194" oldVal="73"/>
+    <row newVal="195" oldVal="236"/>
+    <row newVal="196" oldVal="238"/>
+    <row newVal="197" oldVal="237"/>
+    <row newVal="198" oldVal="91"/>
+    <row newVal="199" oldVal="17"/>
+    <row newVal="200" oldVal="64"/>
+    <row newVal="201" oldVal="77"/>
+    <row newVal="202" oldVal="98"/>
+    <row newVal="203" oldVal="103"/>
+    <row newVal="204" oldVal="202"/>
+    <row newVal="205" oldVal="203"/>
+    <row newVal="206" oldVal="232"/>
+    <row newVal="207" oldVal="96"/>
+    <row newVal="208" oldVal="111"/>
+    <row newVal="209" oldVal="97"/>
+    <row newVal="210" oldVal="24"/>
+    <row newVal="211" oldVal="40"/>
+    <row newVal="212" oldVal="18"/>
+    <row newVal="213" oldVal="48"/>
+    <row newVal="214" oldVal="219"/>
+    <row newVal="215" oldVal="217"/>
+    <row newVal="216" oldVal="4"/>
+    <row newVal="217" oldVal="240"/>
+    <row newVal="218" oldVal="66"/>
+    <row newVal="219" oldVal="230"/>
+    <row newVal="220" oldVal="16"/>
+    <row newVal="221" oldVal="9"/>
+    <row newVal="222" oldVal="35"/>
+    <row newVal="223" oldVal="51"/>
+    <row newVal="224" oldVal="21"/>
+    <row newVal="225" oldVal="74"/>
+    <row newVal="226" oldVal="54"/>
+    <row newVal="227" oldVal="26"/>
+    <row newVal="228" oldVal="43"/>
+    <row newVal="229" oldVal="71"/>
+    <row newVal="230" oldVal="55"/>
+    <row newVal="231" oldVal="212"/>
+    <row newVal="232" oldVal="99"/>
+    <row newVal="233" oldVal="89"/>
+    <row newVal="234" oldVal="105"/>
+    <row newVal="235" oldVal="224"/>
+    <row newVal="236" oldVal="233"/>
+    <row newVal="237" oldVal="112"/>
+    <row newVal="238" oldVal="79"/>
+    <row newVal="239" oldVal="81"/>
+    <row newVal="240" oldVal="90"/>
+  </rowSortMap>
+</worksheetSortMap>
 </file>
</xml_diff>